<commit_message>
Fixed history graph legend.
</commit_message>
<xml_diff>
--- a/src/examples/training/reports/animal_classification_4classes_imbalanced-41fb392e/validation_set.xlsx
+++ b/src/examples/training/reports/animal_classification_4classes_imbalanced-41fb392e/validation_set.xlsx
@@ -461,7 +461,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -481,7 +481,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -501,7 +501,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -521,7 +521,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -541,7 +541,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -561,7 +561,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -581,7 +581,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -601,7 +601,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -621,7 +621,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -641,7 +641,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -661,7 +661,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -681,7 +681,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -701,7 +701,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -721,7 +721,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -741,7 +741,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -761,7 +761,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -781,7 +781,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -801,7 +801,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -821,7 +821,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -841,7 +841,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -861,7 +861,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -881,7 +881,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -901,7 +901,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -921,7 +921,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -941,7 +941,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -961,7 +961,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -981,7 +981,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1001,7 +1001,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1021,7 +1021,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1041,7 +1041,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1061,7 +1061,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1081,7 +1081,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1101,7 +1101,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1121,7 +1121,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1141,7 +1141,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1161,7 +1161,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1181,7 +1181,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1201,7 +1201,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1221,7 +1221,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1241,7 +1241,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1261,7 +1261,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1281,7 +1281,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1301,7 +1301,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1321,7 +1321,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1341,7 +1341,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1361,7 +1361,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1381,7 +1381,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1401,7 +1401,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1421,7 +1421,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -1441,7 +1441,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -1461,7 +1461,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -1481,7 +1481,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1501,7 +1501,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1521,7 +1521,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -1541,7 +1541,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -1561,7 +1561,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -1581,7 +1581,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -1601,7 +1601,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -1621,7 +1621,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -1641,7 +1641,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -1661,7 +1661,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -1681,7 +1681,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -1701,7 +1701,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -1721,7 +1721,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -1741,7 +1741,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -1761,7 +1761,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -1781,7 +1781,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -1801,7 +1801,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -1821,7 +1821,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -1841,7 +1841,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -1861,7 +1861,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -1881,7 +1881,7 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -1901,7 +1901,7 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -1921,7 +1921,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -1941,7 +1941,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -1961,7 +1961,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -1981,7 +1981,7 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -2001,7 +2001,7 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -2021,7 +2021,7 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -2041,7 +2041,7 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>BaseLoader(resize=(128, 128))</t>
+          <t>SimpleLoader(resize=(128, 128))</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">

</xml_diff>